<commit_message>
2023 Jan 4 課堂途中
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F880A924-BC06-49CD-9291-AC60E71D5061}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0126C6-C2B4-4946-9D6F-7AF1F38E1D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>SQL 登入設定 重要！！！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SqlDataReader 原理 只傳Data索引值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL語法 切記不要組合字串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登入程式 寫法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -523,6 +535,35 @@
         <v>10</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>44930</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023 Jan 4 課堂結束
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0126C6-C2B4-4946-9D6F-7AF1F38E1D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E3BAEB-3330-450F-A8A1-82AB9DA1F9D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,26 @@
   </si>
   <si>
     <t>登入程式 寫法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL Injection 寫惡意語法 偷窺 破壞資料 原因: 寫SQL時串接語法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL DateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百元買百雞 練習作業</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找練習題</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防止SQL Injection攻擊</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -564,6 +584,46 @@
         <v>13</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="2">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="2">
+        <v>0.66875000000000007</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="2">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023 Jan 5 課堂結束
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E3BAEB-3330-450F-A8A1-82AB9DA1F9D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85896EB2-A7A7-4540-970D-749FBBFFDEB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,6 +100,14 @@
   </si>
   <si>
     <t>防止SQL Injection攻擊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>講解 Plan //購買百雞計畫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扭蛋機</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -470,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -624,6 +632,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" s="1">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023 Jan 6 課堂途中 有bug
沒有傳到userId
可能要用建構函式傳

也許某處SQL語法有錯
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85896EB2-A7A7-4540-970D-749FBBFFDEB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3322F9C2-5A4C-47DF-87BB-C0CFF84A9556}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +108,26 @@
   </si>
   <si>
     <t>扭蛋機</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code產生器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>const v.s. readonly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>const會在編譯時直接替換成值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Readonly變數只能在建構子給值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -624,7 +644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
         <v>0.68055555555555547</v>
       </c>
@@ -632,12 +652,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>44931</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
         <v>0.42708333333333331</v>
       </c>
@@ -645,12 +665,49 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
         <v>0.6875</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" s="1">
+        <v>44932</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" s="2">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.4">
+      <c r="D49" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 Jan 6 課堂結束
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3322F9C2-5A4C-47DF-87BB-C0CFF84A9556}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114FF8F0-2565-4BE7-996B-6523B919EAC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,6 +128,10 @@
   </si>
   <si>
     <t>Readonly變數只能在建構子給值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重點</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -705,9 +709,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D49" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A50" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 Jan 9 課堂結束
三層式架構
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NewRepoCsharp\ADO.NET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Csharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114FF8F0-2565-4BE7-996B-6523B919EAC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE86A60-B128-4C7A-8F71-BA7574EBA821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>重點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三層式 錯過'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>講故事 錯過</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EditUser</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -502,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -722,6 +734,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A55" s="1">
+        <v>44935</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A56" s="2">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A57" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A58" s="2">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2023 Jan 10 課堂中途
</commit_message>
<xml_diff>
--- a/ADO.NET/ADO.NET_TimeStamp.xlsx
+++ b/ADO.NET/ADO.NET_TimeStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Csharp\ADO.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE86A60-B128-4C7A-8F71-BA7574EBA821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596F0F16-FB2F-47A6-9C11-6AF1E2F5F129}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12320" windowHeight="5760" xr2:uid="{08B4EF31-8FBC-4D9F-9E63-8512BD3BBAC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ADO.NET</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,14 @@
   </si>
   <si>
     <t>EditUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW示範</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>var 匿名物件 介面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,13 +522,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5BDCE0-B976-4A93-9272-9D434E05DAE6}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
@@ -761,6 +772,27 @@
       </c>
       <c r="B58" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A62" s="1">
+        <v>44936</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="B64" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>